<commit_message>
Main form table view
</commit_message>
<xml_diff>
--- a/worksheets/COIN_LIST.xlsx
+++ b/worksheets/COIN_LIST.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>BTC</t>
   </si>
@@ -49,6 +49,276 @@
   </si>
   <si>
     <t>SOL</t>
+  </si>
+  <si>
+    <t>BUSD</t>
+  </si>
+  <si>
+    <t>TRX</t>
+  </si>
+  <si>
+    <t>SHIB</t>
+  </si>
+  <si>
+    <t>UNI</t>
+  </si>
+  <si>
+    <t>AVAX</t>
+  </si>
+  <si>
+    <t>ATOM</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>ETC</t>
+  </si>
+  <si>
+    <t>XMR</t>
+  </si>
+  <si>
+    <t>XLM</t>
+  </si>
+  <si>
+    <t>BCH</t>
+  </si>
+  <si>
+    <t>APE</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>ALGO</t>
+  </si>
+  <si>
+    <t>QNT</t>
+  </si>
+  <si>
+    <t>NEAR</t>
+  </si>
+  <si>
+    <t>VET</t>
+  </si>
+  <si>
+    <t>FIL</t>
+  </si>
+  <si>
+    <t>ICP</t>
+  </si>
+  <si>
+    <t>HBAR</t>
+  </si>
+  <si>
+    <t>EOS</t>
+  </si>
+  <si>
+    <t>LUNC</t>
+  </si>
+  <si>
+    <t>AAVE</t>
+  </si>
+  <si>
+    <t>EGLD</t>
+  </si>
+  <si>
+    <t>THETA</t>
+  </si>
+  <si>
+    <t>FLOW</t>
+  </si>
+  <si>
+    <t>SAND</t>
+  </si>
+  <si>
+    <t>XTZ</t>
+  </si>
+  <si>
+    <t>CHZ</t>
+  </si>
+  <si>
+    <t>AXS</t>
+  </si>
+  <si>
+    <t>MANA</t>
+  </si>
+  <si>
+    <t>ZEC</t>
+  </si>
+  <si>
+    <t>FTM</t>
+  </si>
+  <si>
+    <t>MKR</t>
+  </si>
+  <si>
+    <t>GRT</t>
+  </si>
+  <si>
+    <t>TWT</t>
+  </si>
+  <si>
+    <t>CAKE</t>
+  </si>
+  <si>
+    <t>DASH</t>
+  </si>
+  <si>
+    <t>APT</t>
+  </si>
+  <si>
+    <t>KLAY</t>
+  </si>
+  <si>
+    <t>IOTA</t>
+  </si>
+  <si>
+    <t>PAXG</t>
+  </si>
+  <si>
+    <t>NEO</t>
+  </si>
+  <si>
+    <t>XEC</t>
+  </si>
+  <si>
+    <t>RUNE</t>
+  </si>
+  <si>
+    <t>SNX</t>
+  </si>
+  <si>
+    <t>NEXO</t>
+  </si>
+  <si>
+    <t>FXS</t>
+  </si>
+  <si>
+    <t>ZIL</t>
+  </si>
+  <si>
+    <t>MINA</t>
+  </si>
+  <si>
+    <t>OSMO</t>
+  </si>
+  <si>
+    <t>IMX</t>
+  </si>
+  <si>
+    <t>GMX</t>
+  </si>
+  <si>
+    <t>CRV</t>
+  </si>
+  <si>
+    <t>1INCH</t>
+  </si>
+  <si>
+    <t>STX</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>LRC</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>ENJ</t>
+  </si>
+  <si>
+    <t>DCR</t>
+  </si>
+  <si>
+    <t>XEM</t>
+  </si>
+  <si>
+    <t>KAVA</t>
+  </si>
+  <si>
+    <t>HOT</t>
+  </si>
+  <si>
+    <t>GALA</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>CELO</t>
+  </si>
+  <si>
+    <t>RVN</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>ENS</t>
+  </si>
+  <si>
+    <t>CVX</t>
+  </si>
+  <si>
+    <t>SUSHI</t>
+  </si>
+  <si>
+    <t>IOTX</t>
+  </si>
+  <si>
+    <t>GNO</t>
+  </si>
+  <si>
+    <t>ROSE</t>
+  </si>
+  <si>
+    <t>TFUEL</t>
+  </si>
+  <si>
+    <t>KSM</t>
+  </si>
+  <si>
+    <t>QTUM</t>
+  </si>
+  <si>
+    <t>YFI</t>
+  </si>
+  <si>
+    <t>KDA</t>
+  </si>
+  <si>
+    <t>BNX</t>
+  </si>
+  <si>
+    <t>ANKR</t>
+  </si>
+  <si>
+    <t>GMT</t>
+  </si>
+  <si>
+    <t>WOO</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>JASMY</t>
+  </si>
+  <si>
+    <t>MASK</t>
+  </si>
+  <si>
+    <t>LUNA</t>
+  </si>
+  <si>
+    <t>WAVES</t>
   </si>
 </sst>
 </file>
@@ -366,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +697,456 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>